<commit_message>
Correção dados de documentação e teste
</commit_message>
<xml_diff>
--- a/docs/Orçamento Projeto.xlsx
+++ b/docs/Orçamento Projeto.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luciano\Documents\UFF\2016.2\ES2\Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Visagio\Documents\UFF\ES 2\Trabalho\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Documentação" sheetId="5" r:id="rId5"/>
     <sheet name="Testes" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -220,10 +220,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_-[$R$-416]* #,##0.00_-;\-[$R$-416]* #,##0.00_-;_-[$R$-416]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_-[$R$-416]* #,##0.00_-;\-[$R$-416]* #,##0.00_-;_-[$R$-416]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -399,7 +399,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -433,10 +433,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -451,10 +451,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -463,10 +463,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -475,7 +475,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -484,25 +484,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -827,7 +827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -909,16 +909,16 @@
         <v>56</v>
       </c>
       <c r="C9" s="11">
-        <f>Documentação!B17</f>
-        <v>92</v>
+        <f>Documentação!B20</f>
+        <v>126</v>
       </c>
       <c r="D9" s="14">
-        <f>Documentação!D17</f>
-        <v>1380</v>
+        <f>Documentação!D20</f>
+        <v>1890</v>
       </c>
       <c r="E9" s="14">
-        <f>Documentação!E17</f>
-        <v>1794</v>
+        <f>Documentação!E20</f>
+        <v>2457</v>
       </c>
     </row>
     <row r="10" spans="2:5" s="9" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -927,15 +927,15 @@
       </c>
       <c r="C10" s="11">
         <f>Testes!B17</f>
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="D10" s="14">
         <f>Testes!D17</f>
-        <v>2130</v>
+        <v>1620</v>
       </c>
       <c r="E10" s="14">
         <f>Testes!E17</f>
-        <v>2769</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="C16" s="23"/>
       <c r="D16" s="23">
-        <f t="shared" ref="C16:D16" si="2">SUM(D2:D13)</f>
+        <f t="shared" ref="D16" si="2">SUM(D2:D13)</f>
         <v>615</v>
       </c>
       <c r="E16" s="24">
@@ -1444,7 +1444,7 @@
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="27">
-        <f t="shared" ref="C12:E12" si="2">SUM(D2:D9)</f>
+        <f t="shared" ref="D12:E12" si="2">SUM(D2:D9)</f>
         <v>1275</v>
       </c>
       <c r="E12" s="27">
@@ -1615,7 +1615,7 @@
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="32">
-        <f t="shared" ref="C10:E10" si="2">SUM(D2:D7)</f>
+        <f t="shared" ref="D10:E10" si="2">SUM(D2:D7)</f>
         <v>1605</v>
       </c>
       <c r="E10" s="33">
@@ -1631,10 +1631,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,24 +1909,93 @@
         <v>58.5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:5" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:5" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="34">
+        <v>8</v>
+      </c>
+      <c r="C15" s="35">
+        <v>15</v>
+      </c>
+      <c r="D15" s="35">
+        <f>B15*C15</f>
+        <v>120</v>
+      </c>
+      <c r="E15" s="35">
+        <f>D15*1.3</f>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="34">
+        <v>13</v>
+      </c>
+      <c r="C16" s="35">
+        <v>15</v>
+      </c>
+      <c r="D16" s="35">
+        <f>B16*C16</f>
+        <v>195</v>
+      </c>
+      <c r="E16" s="35">
+        <f>D16*1.3</f>
+        <v>253.5</v>
+      </c>
+    </row>
     <row r="17" spans="1:5" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="34">
+        <v>13</v>
+      </c>
+      <c r="C17" s="35">
+        <v>15</v>
+      </c>
+      <c r="D17" s="35">
+        <f>B17*C17</f>
+        <v>195</v>
+      </c>
+      <c r="E17" s="35">
+        <f>D17*1.3</f>
+        <v>253.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="26">
-        <f>SUM(B2:B14)</f>
-        <v>92</v>
-      </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27">
-        <f t="shared" ref="C17:E17" si="2">SUM(D2:D14)</f>
-        <v>1380</v>
-      </c>
-      <c r="E17" s="36">
-        <f t="shared" si="2"/>
-        <v>1794</v>
+      <c r="B20" s="26">
+        <f>SUM(B2:B17)</f>
+        <v>126</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27">
+        <f>SUM(D2:D17)</f>
+        <v>1890</v>
+      </c>
+      <c r="E20" s="36">
+        <f>SUM(E2:E17)</f>
+        <v>2457</v>
       </c>
     </row>
   </sheetData>
@@ -1939,8 +2008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1997,11 +2066,11 @@
         <v>15</v>
       </c>
       <c r="D3" s="35">
-        <f t="shared" ref="D3:D14" si="0">B3*C3</f>
+        <f>B3*C3</f>
         <v>120</v>
       </c>
       <c r="E3" s="35">
-        <f t="shared" ref="E3:E14" si="1">D3*1.3</f>
+        <f>D3*1.3</f>
         <v>156</v>
       </c>
     </row>
@@ -2016,11 +2085,11 @@
         <v>15</v>
       </c>
       <c r="D4" s="35">
-        <f t="shared" si="0"/>
+        <f>B4*C4</f>
         <v>75</v>
       </c>
       <c r="E4" s="35">
-        <f t="shared" si="1"/>
+        <f>D4*1.3</f>
         <v>97.5</v>
       </c>
     </row>
@@ -2035,11 +2104,11 @@
         <v>15</v>
       </c>
       <c r="D5" s="35">
-        <f t="shared" si="0"/>
+        <f>B5*C5</f>
         <v>75</v>
       </c>
       <c r="E5" s="35">
-        <f t="shared" si="1"/>
+        <f>D5*1.3</f>
         <v>97.5</v>
       </c>
     </row>
@@ -2054,11 +2123,11 @@
         <v>15</v>
       </c>
       <c r="D6" s="35">
-        <f t="shared" si="0"/>
+        <f>B6*C6</f>
         <v>120</v>
       </c>
       <c r="E6" s="35">
-        <f t="shared" si="1"/>
+        <f>D6*1.3</f>
         <v>156</v>
       </c>
     </row>
@@ -2073,11 +2142,11 @@
         <v>15</v>
       </c>
       <c r="D7" s="35">
-        <f t="shared" si="0"/>
+        <f>B7*C7</f>
         <v>120</v>
       </c>
       <c r="E7" s="35">
-        <f t="shared" si="1"/>
+        <f>D7*1.3</f>
         <v>156</v>
       </c>
     </row>
@@ -2092,11 +2161,11 @@
         <v>15</v>
       </c>
       <c r="D8" s="35">
-        <f t="shared" si="0"/>
+        <f>B8*C8</f>
         <v>75</v>
       </c>
       <c r="E8" s="35">
-        <f t="shared" si="1"/>
+        <f>D8*1.3</f>
         <v>97.5</v>
       </c>
     </row>
@@ -2111,11 +2180,11 @@
         <v>15</v>
       </c>
       <c r="D9" s="35">
-        <f t="shared" si="0"/>
+        <f>B9*C9</f>
         <v>600</v>
       </c>
       <c r="E9" s="35">
-        <f t="shared" si="1"/>
+        <f>D9*1.3</f>
         <v>780</v>
       </c>
     </row>
@@ -2130,11 +2199,11 @@
         <v>15</v>
       </c>
       <c r="D10" s="35">
-        <f t="shared" si="0"/>
+        <f>B10*C10</f>
         <v>195</v>
       </c>
       <c r="E10" s="35">
-        <f t="shared" si="1"/>
+        <f>D10*1.3</f>
         <v>253.5</v>
       </c>
     </row>
@@ -2149,71 +2218,17 @@
         <v>15</v>
       </c>
       <c r="D11" s="35">
-        <f t="shared" si="0"/>
+        <f>B11*C11</f>
         <v>120</v>
       </c>
       <c r="E11" s="35">
-        <f t="shared" si="1"/>
+        <f>D11*1.3</f>
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="34">
-        <v>8</v>
-      </c>
-      <c r="C12" s="35">
-        <v>15</v>
-      </c>
-      <c r="D12" s="35">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="E12" s="35">
-        <f t="shared" si="1"/>
-        <v>156</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="34">
-        <v>13</v>
-      </c>
-      <c r="C13" s="35">
-        <v>15</v>
-      </c>
-      <c r="D13" s="35">
-        <f t="shared" si="0"/>
-        <v>195</v>
-      </c>
-      <c r="E13" s="35">
-        <f t="shared" si="1"/>
-        <v>253.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="34">
-        <v>13</v>
-      </c>
-      <c r="C14" s="35">
-        <v>15</v>
-      </c>
-      <c r="D14" s="35">
-        <f t="shared" si="0"/>
-        <v>195</v>
-      </c>
-      <c r="E14" s="35">
-        <f t="shared" si="1"/>
-        <v>253.5</v>
-      </c>
-    </row>
+    <row r="12" spans="1:5" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:5" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:5" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:5" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:5" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:5" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2221,17 +2236,17 @@
         <v>58</v>
       </c>
       <c r="B17" s="26">
-        <f>SUM(B2:B14)</f>
-        <v>142</v>
+        <f>SUM(B2:B11)</f>
+        <v>108</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="27">
-        <f t="shared" ref="C17:E17" si="2">SUM(D2:D14)</f>
-        <v>2130</v>
+        <f>SUM(D2:D11)</f>
+        <v>1620</v>
       </c>
       <c r="E17" s="36">
-        <f t="shared" si="2"/>
-        <v>2769</v>
+        <f>SUM(E2:E11)</f>
+        <v>2106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nova versão do plano de orçamento
Inclusão das reuniões no orçamento
</commit_message>
<xml_diff>
--- a/docs/Orçamento Projeto.xlsx
+++ b/docs/Orçamento Projeto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Geral" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
   <si>
     <t>Tabuleiro (indicando linha e coluna)</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>Reuniões de Planejamento</t>
   </si>
 </sst>
 </file>
@@ -909,16 +912,16 @@
         <v>56</v>
       </c>
       <c r="C9" s="11">
-        <f>Documentação!B20</f>
-        <v>126</v>
+        <f>Documentação!B21</f>
+        <v>144</v>
       </c>
       <c r="D9" s="14">
-        <f>Documentação!D20</f>
-        <v>1890</v>
+        <f>Documentação!D21</f>
+        <v>2160</v>
       </c>
       <c r="E9" s="14">
-        <f>Documentação!E20</f>
-        <v>2457</v>
+        <f>Documentação!E21</f>
+        <v>2808</v>
       </c>
     </row>
     <row r="10" spans="2:5" s="9" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -945,15 +948,15 @@
       </c>
       <c r="C13" s="18">
         <f>SUM(C6:C10)</f>
-        <v>467</v>
+        <v>485</v>
       </c>
       <c r="D13" s="19">
         <f>SUM(D6:D10)</f>
-        <v>7005</v>
+        <v>7275</v>
       </c>
       <c r="E13" s="20">
         <f>SUM(E6:E10)</f>
-        <v>9106.5</v>
+        <v>9457.5</v>
       </c>
     </row>
   </sheetData>
@@ -1631,10 +1634,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,11 +1695,11 @@
         <v>15</v>
       </c>
       <c r="D3" s="35">
-        <f t="shared" ref="D3:D14" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D15" si="0">B3*C3</f>
         <v>75</v>
       </c>
       <c r="E3" s="35">
-        <f t="shared" ref="E3:E14" si="1">D3*1.3</f>
+        <f t="shared" ref="E3:E15" si="1">D3*1.3</f>
         <v>97.5</v>
       </c>
     </row>
@@ -1911,45 +1914,45 @@
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B15" s="34">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C15" s="35">
         <v>15</v>
       </c>
       <c r="D15" s="35">
-        <f>B15*C15</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>270</v>
       </c>
       <c r="E15" s="35">
-        <f>D15*1.3</f>
-        <v>156</v>
+        <f t="shared" si="1"/>
+        <v>351</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="34">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C16" s="35">
         <v>15</v>
       </c>
       <c r="D16" s="35">
         <f>B16*C16</f>
-        <v>195</v>
+        <v>120</v>
       </c>
       <c r="E16" s="35">
         <f>D16*1.3</f>
-        <v>253.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="34">
         <v>13</v>
@@ -1966,14 +1969,26 @@
         <v>253.5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="34">
+        <v>13</v>
+      </c>
+      <c r="C18" s="35">
+        <v>15</v>
+      </c>
+      <c r="D18" s="35">
+        <f>B18*C18</f>
+        <v>195</v>
+      </c>
+      <c r="E18" s="35">
+        <f>D18*1.3</f>
+        <v>253.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1981,21 +1996,28 @@
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="26">
-        <f>SUM(B2:B17)</f>
-        <v>126</v>
-      </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27">
-        <f>SUM(D2:D17)</f>
-        <v>1890</v>
-      </c>
-      <c r="E20" s="36">
-        <f>SUM(E2:E17)</f>
-        <v>2457</v>
+      <c r="B21" s="26">
+        <f>SUM(B2:B18)</f>
+        <v>144</v>
+      </c>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27">
+        <f>SUM(D2:D18)</f>
+        <v>2160</v>
+      </c>
+      <c r="E21" s="36">
+        <f>SUM(E2:E18)</f>
+        <v>2808</v>
       </c>
     </row>
   </sheetData>
@@ -2008,7 +2030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -2047,11 +2069,11 @@
         <v>15</v>
       </c>
       <c r="D2" s="35">
-        <f>B2*C2</f>
+        <f t="shared" ref="D2:D11" si="0">B2*C2</f>
         <v>120</v>
       </c>
       <c r="E2" s="35">
-        <f>D2*1.3</f>
+        <f t="shared" ref="E2:E11" si="1">D2*1.3</f>
         <v>156</v>
       </c>
     </row>
@@ -2066,11 +2088,11 @@
         <v>15</v>
       </c>
       <c r="D3" s="35">
-        <f>B3*C3</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="E3" s="35">
-        <f>D3*1.3</f>
+        <f t="shared" si="1"/>
         <v>156</v>
       </c>
     </row>
@@ -2085,11 +2107,11 @@
         <v>15</v>
       </c>
       <c r="D4" s="35">
-        <f>B4*C4</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="E4" s="35">
-        <f>D4*1.3</f>
+        <f t="shared" si="1"/>
         <v>97.5</v>
       </c>
     </row>
@@ -2104,11 +2126,11 @@
         <v>15</v>
       </c>
       <c r="D5" s="35">
-        <f>B5*C5</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="E5" s="35">
-        <f>D5*1.3</f>
+        <f t="shared" si="1"/>
         <v>97.5</v>
       </c>
     </row>
@@ -2123,11 +2145,11 @@
         <v>15</v>
       </c>
       <c r="D6" s="35">
-        <f>B6*C6</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="E6" s="35">
-        <f>D6*1.3</f>
+        <f t="shared" si="1"/>
         <v>156</v>
       </c>
     </row>
@@ -2142,11 +2164,11 @@
         <v>15</v>
       </c>
       <c r="D7" s="35">
-        <f>B7*C7</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="E7" s="35">
-        <f>D7*1.3</f>
+        <f t="shared" si="1"/>
         <v>156</v>
       </c>
     </row>
@@ -2161,11 +2183,11 @@
         <v>15</v>
       </c>
       <c r="D8" s="35">
-        <f>B8*C8</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="E8" s="35">
-        <f>D8*1.3</f>
+        <f t="shared" si="1"/>
         <v>97.5</v>
       </c>
     </row>
@@ -2180,11 +2202,11 @@
         <v>15</v>
       </c>
       <c r="D9" s="35">
-        <f>B9*C9</f>
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="E9" s="35">
-        <f>D9*1.3</f>
+        <f t="shared" si="1"/>
         <v>780</v>
       </c>
     </row>
@@ -2199,11 +2221,11 @@
         <v>15</v>
       </c>
       <c r="D10" s="35">
-        <f>B10*C10</f>
+        <f t="shared" si="0"/>
         <v>195</v>
       </c>
       <c r="E10" s="35">
-        <f>D10*1.3</f>
+        <f t="shared" si="1"/>
         <v>253.5</v>
       </c>
     </row>
@@ -2218,11 +2240,11 @@
         <v>15</v>
       </c>
       <c r="D11" s="35">
-        <f>B11*C11</f>
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="E11" s="35">
-        <f>D11*1.3</f>
+        <f t="shared" si="1"/>
         <v>156</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correção de cálculos de reunião
</commit_message>
<xml_diff>
--- a/docs/Orçamento Projeto.xlsx
+++ b/docs/Orçamento Projeto.xlsx
@@ -913,15 +913,15 @@
       </c>
       <c r="C9" s="11">
         <f>Documentação!B21</f>
-        <v>144</v>
+        <v>234</v>
       </c>
       <c r="D9" s="14">
         <f>Documentação!D21</f>
-        <v>2160</v>
+        <v>3510</v>
       </c>
       <c r="E9" s="14">
         <f>Documentação!E21</f>
-        <v>2808</v>
+        <v>4563</v>
       </c>
     </row>
     <row r="10" spans="2:5" s="9" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -948,15 +948,15 @@
       </c>
       <c r="C13" s="18">
         <f>SUM(C6:C10)</f>
-        <v>485</v>
+        <v>575</v>
       </c>
       <c r="D13" s="19">
         <f>SUM(D6:D10)</f>
-        <v>7275</v>
+        <v>8625</v>
       </c>
       <c r="E13" s="20">
         <f>SUM(E6:E10)</f>
-        <v>9457.5</v>
+        <v>11212.5</v>
       </c>
     </row>
   </sheetData>
@@ -1637,7 +1637,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1917,18 +1917,18 @@
         <v>62</v>
       </c>
       <c r="B15" s="34">
-        <v>18</v>
+        <v>108</v>
       </c>
       <c r="C15" s="35">
         <v>15</v>
       </c>
       <c r="D15" s="35">
         <f t="shared" si="0"/>
-        <v>270</v>
+        <v>1620</v>
       </c>
       <c r="E15" s="35">
         <f t="shared" si="1"/>
-        <v>351</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2008,16 +2008,16 @@
       </c>
       <c r="B21" s="26">
         <f>SUM(B2:B18)</f>
-        <v>144</v>
+        <v>234</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="27">
         <f>SUM(D2:D18)</f>
-        <v>2160</v>
+        <v>3510</v>
       </c>
       <c r="E21" s="36">
         <f>SUM(E2:E18)</f>
-        <v>2808</v>
+        <v>4563</v>
       </c>
     </row>
   </sheetData>

</xml_diff>